<commit_message>
modif px et img logo
</commit_message>
<xml_diff>
--- a/AXE D AMELIORATION.xlsx
+++ b/AXE D AMELIORATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\p4\p4\La-chouette-agence-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{834EB00B-53D7-4D0A-AF3E-C15851B5C3BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A65F8E-B41E-4FDC-9DF6-6C6542123B04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{9C8A9F05-E235-4987-8102-7AA14F5BF94F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Axe d'amélioration</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Modification des liens du script page 2</t>
+  </si>
+  <si>
+    <t>Ajout d'une couleur au survol pour les liens accueil et contact</t>
+  </si>
+  <si>
+    <t>suppression des img de citation et modification en texte</t>
+  </si>
+  <si>
+    <t>Modification du footer en mettant des infos utile</t>
   </si>
 </sst>
 </file>
@@ -409,239 +418,255 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
modif débordement div row
</commit_message>
<xml_diff>
--- a/AXE D AMELIORATION.xlsx
+++ b/AXE D AMELIORATION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mouatakide1\Desktop\p4\p4\La-chouette-agence-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A65F8E-B41E-4FDC-9DF6-6C6542123B04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8543AF-F313-48FC-978D-E8FA1A37320D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="150" yWindow="0" windowWidth="19050" windowHeight="14760" xr2:uid="{9C8A9F05-E235-4987-8102-7AA14F5BF94F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Axe d'amélioration</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Modification du footer en mettant des infos utile</t>
+  </si>
+  <si>
+    <t>Modification de la div row padding a 0px pour ne pas que la div dépasse</t>
+  </si>
+  <si>
+    <t>suppresion du css dans l'html</t>
+  </si>
+  <si>
+    <t>Modification des différentes parti du htlm</t>
   </si>
 </sst>
 </file>
@@ -418,12 +427,12 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="55.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -531,21 +540,39 @@
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>